<commit_message>
Updating SDTM annotations on draft Collection DSS
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_EG_Local.xlsx
+++ b/curation/draft/collection/collection_specialization_EG_Local.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\collection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD59482-7F02-4946-9093-7A46EC8C6CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBD8E39-7563-48F6-B947-F75742F89B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_EG!$A$1:$AG$81</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="213">
   <si>
     <t>package_date</t>
   </si>
@@ -299,9 +299,6 @@
     <t>EGORRESU; EGTEST; EGTESTCD</t>
   </si>
   <si>
-    <t>EGORRESU when EGTESTCD = EGHRMN</t>
-  </si>
-  <si>
     <t>C117779</t>
   </si>
   <si>
@@ -641,9 +638,6 @@
     <t>12 LEAD STANDARD</t>
   </si>
   <si>
-    <t>12 Lead Standard</t>
-  </si>
-  <si>
     <t>C82525</t>
   </si>
   <si>
@@ -657,6 +651,33 @@
   </si>
   <si>
     <t>Position</t>
+  </si>
+  <si>
+    <t>C71102</t>
+  </si>
+  <si>
+    <t>EGMETHOD = 12 LEAD STANDARD when EGTESTCD = EGHRMN</t>
+  </si>
+  <si>
+    <t>EGMETHOD = 12 LEAD STANDARD when EGTESTCD = QRSAG</t>
+  </si>
+  <si>
+    <t>EGMETHOD = 12 LEAD STANDARD when EGTESTCD = PRAG</t>
+  </si>
+  <si>
+    <t>EGMETHOD = 12 LEAD STANDARD when EGTESTCD = QTAG</t>
+  </si>
+  <si>
+    <t>EGMETHOD = 12 LEAD STANDARD when EGTESTCD = QTCBAG</t>
+  </si>
+  <si>
+    <t>EGMETHOD = 12 LEAD STANDARD when EGTESTCD = QTCFAG</t>
+  </si>
+  <si>
+    <t>EGMETHOD = 12 LEAD STANDARD when EGTESTCD = QTCUNSAG</t>
+  </si>
+  <si>
+    <t>EGORRESU = beats/min when EGTESTCD = EGHRMN</t>
   </si>
 </sst>
 </file>
@@ -1061,29 +1082,34 @@
   <dimension ref="A1:AG81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="AE74" sqref="AE74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="10" max="10" width="30" customWidth="1"/>
-    <col min="11" max="11" width="29.85546875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="18" customWidth="1"/>
-    <col min="15" max="15" width="31.42578125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="26.28515625" customWidth="1"/>
-    <col min="20" max="20" width="14.140625" customWidth="1"/>
-    <col min="21" max="21" width="24.140625" customWidth="1"/>
-    <col min="22" max="22" width="21" customWidth="1"/>
-    <col min="24" max="24" width="19.7109375" customWidth="1"/>
-    <col min="25" max="25" width="21.7109375" style="3" customWidth="1"/>
-    <col min="26" max="26" width="22" style="3" customWidth="1"/>
-    <col min="27" max="27" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="30" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="29.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="12" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="18" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="31.42578125" style="3" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="26.28515625" hidden="1" customWidth="1"/>
+    <col min="17" max="19" width="0" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="14.140625" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="24.140625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="21" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="0" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="19.7109375" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="21.7109375" style="3" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="22" style="3" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="15.140625" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="19.85546875" customWidth="1"/>
     <col min="29" max="29" width="21.85546875" customWidth="1"/>
-    <col min="30" max="30" width="22.140625" style="3" customWidth="1"/>
-    <col min="31" max="31" width="30.42578125" style="3" customWidth="1"/>
+    <col min="30" max="30" width="24.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="74.42578125" style="3" customWidth="1"/>
     <col min="32" max="32" width="16" customWidth="1"/>
     <col min="33" max="33" width="12.85546875" customWidth="1"/>
   </cols>
@@ -1191,7 +1217,7 @@
     </row>
     <row r="2" spans="1:33" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D2" t="s">
         <v>33</v>
@@ -1215,7 +1241,7 @@
         <v>36</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>38</v>
@@ -1253,7 +1279,7 @@
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D3" t="s">
         <v>33</v>
@@ -1360,7 +1386,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>53</v>
       </c>
@@ -1418,20 +1444,17 @@
       <c r="X5" t="s">
         <v>60</v>
       </c>
-      <c r="Y5" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z5" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>45</v>
+      <c r="AB5" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>204</v>
       </c>
       <c r="AD5" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>60</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="45" x14ac:dyDescent="0.25">
@@ -1636,27 +1659,27 @@
         <v>85</v>
       </c>
       <c r="AE8" s="3" t="s">
-        <v>86</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
         <v>87</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" t="s">
         <v>88</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" t="s">
-        <v>89</v>
       </c>
       <c r="I9" t="s">
         <v>56</v>
@@ -1665,7 +1688,7 @@
         <v>57</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L9" t="s">
         <v>47</v>
@@ -1698,24 +1721,24 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
         <v>87</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
         <v>88</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" t="s">
-        <v>89</v>
       </c>
       <c r="I10" t="s">
         <v>56</v>
@@ -1724,7 +1747,7 @@
         <v>57</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L10" t="s">
         <v>60</v>
@@ -1756,40 +1779,37 @@
       <c r="X10" t="s">
         <v>60</v>
       </c>
-      <c r="Y10" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z10" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>45</v>
+      <c r="AB10" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>204</v>
       </c>
       <c r="AD10" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AE10" s="3" t="s">
-        <v>60</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:33" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" t="s">
         <v>87</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" t="s">
         <v>88</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" t="s">
-        <v>89</v>
       </c>
       <c r="I11" t="s">
         <v>56</v>
@@ -1798,7 +1818,7 @@
         <v>57</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L11" t="s">
         <v>64</v>
@@ -1848,22 +1868,22 @@
     </row>
     <row r="12" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" t="s">
         <v>87</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" t="s">
         <v>88</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" t="s">
-        <v>89</v>
       </c>
       <c r="I12" t="s">
         <v>56</v>
@@ -1872,19 +1892,19 @@
         <v>57</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M12" t="s">
         <v>71</v>
       </c>
       <c r="N12" t="s">
+        <v>90</v>
+      </c>
+      <c r="O12" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="Q12">
         <v>4</v>
@@ -1902,27 +1922,27 @@
         <v>75</v>
       </c>
       <c r="AE12" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" t="s">
         <v>87</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" t="s">
         <v>88</v>
-      </c>
-      <c r="D13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" t="s">
-        <v>89</v>
       </c>
       <c r="I13" t="s">
         <v>56</v>
@@ -1931,19 +1951,19 @@
         <v>57</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M13" t="s">
         <v>78</v>
       </c>
       <c r="N13" t="s">
+        <v>94</v>
+      </c>
+      <c r="O13" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="Q13">
         <v>5</v>
@@ -1964,10 +1984,10 @@
         <v>82</v>
       </c>
       <c r="Y13" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z13" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="Z13" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="AA13" t="s">
         <v>45</v>
@@ -1976,27 +1996,27 @@
         <v>85</v>
       </c>
       <c r="AE13" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" t="s">
         <v>100</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" t="s">
         <v>101</v>
-      </c>
-      <c r="D14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" t="s">
-        <v>102</v>
       </c>
       <c r="I14" t="s">
         <v>56</v>
@@ -2005,7 +2025,7 @@
         <v>57</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L14" t="s">
         <v>47</v>
@@ -2038,24 +2058,24 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" t="s">
         <v>100</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" t="s">
         <v>101</v>
-      </c>
-      <c r="D15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" t="s">
-        <v>35</v>
-      </c>
-      <c r="H15" t="s">
-        <v>102</v>
       </c>
       <c r="I15" t="s">
         <v>56</v>
@@ -2064,7 +2084,7 @@
         <v>57</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L15" t="s">
         <v>60</v>
@@ -2096,40 +2116,37 @@
       <c r="X15" t="s">
         <v>60</v>
       </c>
-      <c r="Y15" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z15" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>45</v>
+      <c r="AB15" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>204</v>
       </c>
       <c r="AD15" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AE15" s="3" t="s">
-        <v>60</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:33" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" t="s">
         <v>100</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" t="s">
         <v>101</v>
-      </c>
-      <c r="D16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" t="s">
-        <v>35</v>
-      </c>
-      <c r="H16" t="s">
-        <v>102</v>
       </c>
       <c r="I16" t="s">
         <v>56</v>
@@ -2138,7 +2155,7 @@
         <v>57</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L16" t="s">
         <v>64</v>
@@ -2188,22 +2205,22 @@
     </row>
     <row r="17" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" t="s">
         <v>100</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" t="s">
         <v>101</v>
-      </c>
-      <c r="D17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" t="s">
-        <v>102</v>
       </c>
       <c r="I17" t="s">
         <v>56</v>
@@ -2212,19 +2229,19 @@
         <v>57</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M17" t="s">
         <v>71</v>
       </c>
       <c r="N17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q17">
         <v>4</v>
@@ -2242,27 +2259,27 @@
         <v>75</v>
       </c>
       <c r="AE17" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" t="s">
         <v>100</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" t="s">
         <v>101</v>
-      </c>
-      <c r="D18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" t="s">
-        <v>35</v>
-      </c>
-      <c r="H18" t="s">
-        <v>102</v>
       </c>
       <c r="I18" t="s">
         <v>56</v>
@@ -2271,19 +2288,19 @@
         <v>57</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M18" t="s">
         <v>78</v>
       </c>
       <c r="N18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q18">
         <v>5</v>
@@ -2304,10 +2321,10 @@
         <v>82</v>
       </c>
       <c r="Y18" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z18" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="Z18" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="AA18" t="s">
         <v>45</v>
@@ -2316,27 +2333,27 @@
         <v>85</v>
       </c>
       <c r="AE18" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" t="s">
         <v>109</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" t="s">
         <v>110</v>
-      </c>
-      <c r="D19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19" t="s">
-        <v>111</v>
       </c>
       <c r="I19" t="s">
         <v>56</v>
@@ -2345,7 +2362,7 @@
         <v>57</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L19" t="s">
         <v>47</v>
@@ -2380,22 +2397,22 @@
     </row>
     <row r="20" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" t="s">
         <v>109</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" t="s">
         <v>110</v>
-      </c>
-      <c r="D20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20" t="s">
-        <v>111</v>
       </c>
       <c r="I20" t="s">
         <v>56</v>
@@ -2404,7 +2421,7 @@
         <v>57</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L20" t="s">
         <v>60</v>
@@ -2436,40 +2453,37 @@
       <c r="X20" t="s">
         <v>60</v>
       </c>
-      <c r="Y20" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z20" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>45</v>
+      <c r="AB20" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>204</v>
       </c>
       <c r="AD20" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AE20" s="3" t="s">
-        <v>60</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="2:31" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" t="s">
         <v>109</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" t="s">
         <v>110</v>
-      </c>
-      <c r="D21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" t="s">
-        <v>35</v>
-      </c>
-      <c r="H21" t="s">
-        <v>111</v>
       </c>
       <c r="I21" t="s">
         <v>56</v>
@@ -2478,7 +2492,7 @@
         <v>57</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L21" t="s">
         <v>64</v>
@@ -2528,22 +2542,22 @@
     </row>
     <row r="22" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" t="s">
         <v>109</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" t="s">
         <v>110</v>
-      </c>
-      <c r="D22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" t="s">
-        <v>111</v>
       </c>
       <c r="I22" t="s">
         <v>56</v>
@@ -2552,19 +2566,19 @@
         <v>57</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M22" t="s">
         <v>71</v>
       </c>
       <c r="N22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q22">
         <v>4</v>
@@ -2582,27 +2596,27 @@
         <v>75</v>
       </c>
       <c r="AE22" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" t="s">
         <v>109</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" t="s">
         <v>110</v>
-      </c>
-      <c r="D23" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" t="s">
-        <v>35</v>
-      </c>
-      <c r="H23" t="s">
-        <v>111</v>
       </c>
       <c r="I23" t="s">
         <v>56</v>
@@ -2611,19 +2625,19 @@
         <v>57</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M23" t="s">
         <v>78</v>
       </c>
       <c r="N23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q23">
         <v>5</v>
@@ -2644,10 +2658,10 @@
         <v>82</v>
       </c>
       <c r="Y23" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z23" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="Z23" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="AA23" t="s">
         <v>45</v>
@@ -2656,27 +2670,27 @@
         <v>85</v>
       </c>
       <c r="AE23" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" t="s">
         <v>118</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" t="s">
         <v>119</v>
-      </c>
-      <c r="D24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" t="s">
-        <v>35</v>
-      </c>
-      <c r="H24" t="s">
-        <v>120</v>
       </c>
       <c r="I24" t="s">
         <v>56</v>
@@ -2685,7 +2699,7 @@
         <v>57</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L24" t="s">
         <v>47</v>
@@ -2720,22 +2734,22 @@
     </row>
     <row r="25" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" t="s">
         <v>118</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" t="s">
+        <v>35</v>
+      </c>
+      <c r="H25" t="s">
         <v>119</v>
-      </c>
-      <c r="D25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" t="s">
-        <v>35</v>
-      </c>
-      <c r="H25" t="s">
-        <v>120</v>
       </c>
       <c r="I25" t="s">
         <v>56</v>
@@ -2744,7 +2758,7 @@
         <v>57</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L25" t="s">
         <v>60</v>
@@ -2776,40 +2790,37 @@
       <c r="X25" t="s">
         <v>60</v>
       </c>
-      <c r="Y25" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z25" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>45</v>
+      <c r="AB25" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>204</v>
       </c>
       <c r="AD25" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AE25" s="3" t="s">
-        <v>60</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="2:31" ht="45" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" t="s">
         <v>118</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" t="s">
         <v>119</v>
-      </c>
-      <c r="D26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" t="s">
-        <v>35</v>
-      </c>
-      <c r="H26" t="s">
-        <v>120</v>
       </c>
       <c r="I26" t="s">
         <v>56</v>
@@ -2818,7 +2829,7 @@
         <v>57</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L26" t="s">
         <v>64</v>
@@ -2868,22 +2879,22 @@
     </row>
     <row r="27" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" t="s">
         <v>118</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" t="s">
         <v>119</v>
-      </c>
-      <c r="D27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" t="s">
-        <v>35</v>
-      </c>
-      <c r="H27" t="s">
-        <v>120</v>
       </c>
       <c r="I27" t="s">
         <v>56</v>
@@ -2892,19 +2903,19 @@
         <v>57</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M27" t="s">
         <v>71</v>
       </c>
       <c r="N27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O27" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q27">
         <v>4</v>
@@ -2922,27 +2933,27 @@
         <v>75</v>
       </c>
       <c r="AE27" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" t="s">
         <v>118</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H28" t="s">
         <v>119</v>
-      </c>
-      <c r="D28" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" t="s">
-        <v>34</v>
-      </c>
-      <c r="G28" t="s">
-        <v>35</v>
-      </c>
-      <c r="H28" t="s">
-        <v>120</v>
       </c>
       <c r="I28" t="s">
         <v>56</v>
@@ -2951,19 +2962,19 @@
         <v>57</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M28" t="s">
         <v>78</v>
       </c>
       <c r="N28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q28">
         <v>5</v>
@@ -2984,10 +2995,10 @@
         <v>82</v>
       </c>
       <c r="Y28" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z28" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="Z28" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="AA28" t="s">
         <v>45</v>
@@ -2996,27 +3007,27 @@
         <v>85</v>
       </c>
       <c r="AE28" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" t="s">
         <v>127</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" t="s">
+        <v>35</v>
+      </c>
+      <c r="H29" t="s">
         <v>128</v>
-      </c>
-      <c r="D29" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" t="s">
-        <v>34</v>
-      </c>
-      <c r="G29" t="s">
-        <v>35</v>
-      </c>
-      <c r="H29" t="s">
-        <v>129</v>
       </c>
       <c r="I29" t="s">
         <v>56</v>
@@ -3025,7 +3036,7 @@
         <v>57</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L29" t="s">
         <v>47</v>
@@ -3060,22 +3071,22 @@
     </row>
     <row r="30" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" t="s">
         <v>127</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30" t="s">
         <v>128</v>
-      </c>
-      <c r="D30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" t="s">
-        <v>34</v>
-      </c>
-      <c r="G30" t="s">
-        <v>35</v>
-      </c>
-      <c r="H30" t="s">
-        <v>129</v>
       </c>
       <c r="I30" t="s">
         <v>56</v>
@@ -3084,7 +3095,7 @@
         <v>57</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L30" t="s">
         <v>60</v>
@@ -3116,40 +3127,37 @@
       <c r="X30" t="s">
         <v>60</v>
       </c>
-      <c r="Y30" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z30" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>45</v>
+      <c r="AB30" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>204</v>
       </c>
       <c r="AD30" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AE30" s="3" t="s">
-        <v>60</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="2:31" ht="45" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" t="s">
         <v>127</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" t="s">
         <v>128</v>
-      </c>
-      <c r="D31" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" t="s">
-        <v>34</v>
-      </c>
-      <c r="G31" t="s">
-        <v>35</v>
-      </c>
-      <c r="H31" t="s">
-        <v>129</v>
       </c>
       <c r="I31" t="s">
         <v>56</v>
@@ -3158,7 +3166,7 @@
         <v>57</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L31" t="s">
         <v>64</v>
@@ -3208,22 +3216,22 @@
     </row>
     <row r="32" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" t="s">
         <v>127</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" t="s">
         <v>128</v>
-      </c>
-      <c r="D32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" t="s">
-        <v>34</v>
-      </c>
-      <c r="G32" t="s">
-        <v>35</v>
-      </c>
-      <c r="H32" t="s">
-        <v>129</v>
       </c>
       <c r="I32" t="s">
         <v>56</v>
@@ -3232,19 +3240,19 @@
         <v>57</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M32" t="s">
         <v>71</v>
       </c>
       <c r="N32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q32">
         <v>4</v>
@@ -3262,27 +3270,27 @@
         <v>75</v>
       </c>
       <c r="AE32" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" t="s">
         <v>127</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" t="s">
+        <v>35</v>
+      </c>
+      <c r="H33" t="s">
         <v>128</v>
-      </c>
-      <c r="D33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E33" t="s">
-        <v>34</v>
-      </c>
-      <c r="G33" t="s">
-        <v>35</v>
-      </c>
-      <c r="H33" t="s">
-        <v>129</v>
       </c>
       <c r="I33" t="s">
         <v>56</v>
@@ -3291,19 +3299,19 @@
         <v>57</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M33" t="s">
         <v>78</v>
       </c>
       <c r="N33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q33">
         <v>5</v>
@@ -3324,10 +3332,10 @@
         <v>82</v>
       </c>
       <c r="Y33" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z33" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="Z33" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="AA33" t="s">
         <v>45</v>
@@ -3336,27 +3344,27 @@
         <v>85</v>
       </c>
       <c r="AE33" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" t="s">
         <v>136</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" t="s">
+        <v>35</v>
+      </c>
+      <c r="H34" t="s">
         <v>137</v>
-      </c>
-      <c r="D34" t="s">
-        <v>33</v>
-      </c>
-      <c r="E34" t="s">
-        <v>34</v>
-      </c>
-      <c r="G34" t="s">
-        <v>35</v>
-      </c>
-      <c r="H34" t="s">
-        <v>138</v>
       </c>
       <c r="I34" t="s">
         <v>56</v>
@@ -3365,7 +3373,7 @@
         <v>57</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L34" t="s">
         <v>47</v>
@@ -3400,22 +3408,22 @@
     </row>
     <row r="35" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35" t="s">
         <v>136</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" t="s">
+        <v>35</v>
+      </c>
+      <c r="H35" t="s">
         <v>137</v>
-      </c>
-      <c r="D35" t="s">
-        <v>33</v>
-      </c>
-      <c r="E35" t="s">
-        <v>34</v>
-      </c>
-      <c r="G35" t="s">
-        <v>35</v>
-      </c>
-      <c r="H35" t="s">
-        <v>138</v>
       </c>
       <c r="I35" t="s">
         <v>56</v>
@@ -3424,7 +3432,7 @@
         <v>57</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L35" t="s">
         <v>60</v>
@@ -3456,40 +3464,37 @@
       <c r="X35" t="s">
         <v>60</v>
       </c>
-      <c r="Y35" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z35" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA35" t="s">
-        <v>45</v>
+      <c r="AB35" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>204</v>
       </c>
       <c r="AD35" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AE35" s="3" t="s">
-        <v>60</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36" spans="2:31" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" t="s">
         <v>136</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" t="s">
+        <v>35</v>
+      </c>
+      <c r="H36" t="s">
         <v>137</v>
-      </c>
-      <c r="D36" t="s">
-        <v>33</v>
-      </c>
-      <c r="E36" t="s">
-        <v>34</v>
-      </c>
-      <c r="G36" t="s">
-        <v>35</v>
-      </c>
-      <c r="H36" t="s">
-        <v>138</v>
       </c>
       <c r="I36" t="s">
         <v>56</v>
@@ -3498,7 +3503,7 @@
         <v>57</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L36" t="s">
         <v>64</v>
@@ -3548,22 +3553,22 @@
     </row>
     <row r="37" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" t="s">
         <v>136</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" t="s">
+        <v>34</v>
+      </c>
+      <c r="G37" t="s">
+        <v>35</v>
+      </c>
+      <c r="H37" t="s">
         <v>137</v>
-      </c>
-      <c r="D37" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" t="s">
-        <v>34</v>
-      </c>
-      <c r="G37" t="s">
-        <v>35</v>
-      </c>
-      <c r="H37" t="s">
-        <v>138</v>
       </c>
       <c r="I37" t="s">
         <v>56</v>
@@ -3572,19 +3577,19 @@
         <v>57</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M37" t="s">
         <v>71</v>
       </c>
       <c r="N37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q37">
         <v>4</v>
@@ -3602,27 +3607,27 @@
         <v>75</v>
       </c>
       <c r="AE37" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>135</v>
+      </c>
+      <c r="C38" t="s">
         <v>136</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" t="s">
+        <v>34</v>
+      </c>
+      <c r="G38" t="s">
+        <v>35</v>
+      </c>
+      <c r="H38" t="s">
         <v>137</v>
-      </c>
-      <c r="D38" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" t="s">
-        <v>34</v>
-      </c>
-      <c r="G38" t="s">
-        <v>35</v>
-      </c>
-      <c r="H38" t="s">
-        <v>138</v>
       </c>
       <c r="I38" t="s">
         <v>56</v>
@@ -3631,19 +3636,19 @@
         <v>57</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M38" t="s">
         <v>78</v>
       </c>
       <c r="N38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q38">
         <v>5</v>
@@ -3664,10 +3669,10 @@
         <v>82</v>
       </c>
       <c r="Y38" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z38" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="Z38" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="AA38" t="s">
         <v>45</v>
@@ -3676,27 +3681,27 @@
         <v>85</v>
       </c>
       <c r="AE38" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
+        <v>144</v>
+      </c>
+      <c r="C39" t="s">
         <v>145</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" t="s">
+        <v>34</v>
+      </c>
+      <c r="G39" t="s">
+        <v>35</v>
+      </c>
+      <c r="H39" t="s">
         <v>146</v>
-      </c>
-      <c r="D39" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" t="s">
-        <v>34</v>
-      </c>
-      <c r="G39" t="s">
-        <v>35</v>
-      </c>
-      <c r="H39" t="s">
-        <v>147</v>
       </c>
       <c r="I39" t="s">
         <v>56</v>
@@ -3705,7 +3710,7 @@
         <v>57</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L39" t="s">
         <v>47</v>
@@ -3740,22 +3745,22 @@
     </row>
     <row r="40" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
+        <v>144</v>
+      </c>
+      <c r="C40" t="s">
         <v>145</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E40" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" t="s">
+        <v>35</v>
+      </c>
+      <c r="H40" t="s">
         <v>146</v>
-      </c>
-      <c r="D40" t="s">
-        <v>33</v>
-      </c>
-      <c r="E40" t="s">
-        <v>34</v>
-      </c>
-      <c r="G40" t="s">
-        <v>35</v>
-      </c>
-      <c r="H40" t="s">
-        <v>147</v>
       </c>
       <c r="I40" t="s">
         <v>56</v>
@@ -3764,19 +3769,19 @@
         <v>57</v>
       </c>
       <c r="K40" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="L40" t="s">
         <v>148</v>
-      </c>
-      <c r="L40" t="s">
-        <v>149</v>
       </c>
       <c r="M40" t="s">
         <v>71</v>
       </c>
       <c r="N40" t="s">
+        <v>149</v>
+      </c>
+      <c r="O40" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="O40" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="Q40">
         <v>2</v>
@@ -3791,16 +3796,16 @@
         <v>3</v>
       </c>
       <c r="W40" t="s">
+        <v>151</v>
+      </c>
+      <c r="X40" t="s">
         <v>152</v>
       </c>
-      <c r="X40" t="s">
+      <c r="Y40" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="Y40" s="3" t="s">
+      <c r="Z40" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="Z40" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="AA40" t="s">
         <v>45</v>
@@ -3809,27 +3814,27 @@
         <v>75</v>
       </c>
       <c r="AE40" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
+        <v>144</v>
+      </c>
+      <c r="C41" t="s">
         <v>145</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" t="s">
+        <v>34</v>
+      </c>
+      <c r="G41" t="s">
+        <v>35</v>
+      </c>
+      <c r="H41" t="s">
         <v>146</v>
-      </c>
-      <c r="D41" t="s">
-        <v>33</v>
-      </c>
-      <c r="E41" t="s">
-        <v>34</v>
-      </c>
-      <c r="G41" t="s">
-        <v>35</v>
-      </c>
-      <c r="H41" t="s">
-        <v>147</v>
       </c>
       <c r="I41" t="s">
         <v>56</v>
@@ -3838,19 +3843,19 @@
         <v>57</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L41" t="s">
+        <v>156</v>
+      </c>
+      <c r="M41" t="s">
+        <v>156</v>
+      </c>
+      <c r="N41" t="s">
         <v>157</v>
       </c>
-      <c r="M41" t="s">
-        <v>157</v>
-      </c>
-      <c r="N41" t="s">
+      <c r="O41" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="O41" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="Q41">
         <v>3</v>
@@ -3880,30 +3885,30 @@
         <v>45</v>
       </c>
       <c r="AD41" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AE41" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="2:31" ht="75" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
+        <v>144</v>
+      </c>
+      <c r="C42" t="s">
         <v>145</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" t="s">
+        <v>34</v>
+      </c>
+      <c r="G42" t="s">
+        <v>35</v>
+      </c>
+      <c r="H42" t="s">
         <v>146</v>
-      </c>
-      <c r="D42" t="s">
-        <v>33</v>
-      </c>
-      <c r="E42" t="s">
-        <v>34</v>
-      </c>
-      <c r="G42" t="s">
-        <v>35</v>
-      </c>
-      <c r="H42" t="s">
-        <v>147</v>
       </c>
       <c r="I42" t="s">
         <v>56</v>
@@ -3912,19 +3917,19 @@
         <v>57</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L42" t="s">
+        <v>159</v>
+      </c>
+      <c r="M42" t="s">
+        <v>159</v>
+      </c>
+      <c r="N42" t="s">
         <v>160</v>
       </c>
-      <c r="M42" t="s">
-        <v>160</v>
-      </c>
-      <c r="N42" t="s">
+      <c r="O42" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="O42" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="Q42">
         <v>4</v>
@@ -3939,25 +3944,25 @@
         <v>50</v>
       </c>
       <c r="W42" t="s">
+        <v>162</v>
+      </c>
+      <c r="X42" t="s">
         <v>163</v>
       </c>
-      <c r="X42" t="s">
-        <v>164</v>
-      </c>
       <c r="Y42" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="Z42" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AA42" t="s">
         <v>45</v>
       </c>
       <c r="AD42" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AE42" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="2:31" ht="30" x14ac:dyDescent="0.25">
@@ -3977,16 +3982,16 @@
         <v>35</v>
       </c>
       <c r="H43" t="s">
+        <v>164</v>
+      </c>
+      <c r="I43" t="s">
         <v>165</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
+        <v>57</v>
+      </c>
+      <c r="K43" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="J43" t="s">
-        <v>57</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="L43" t="s">
         <v>47</v>
@@ -4036,16 +4041,16 @@
         <v>35</v>
       </c>
       <c r="H44" t="s">
+        <v>164</v>
+      </c>
+      <c r="I44" t="s">
         <v>165</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
+        <v>57</v>
+      </c>
+      <c r="K44" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="J44" t="s">
-        <v>57</v>
-      </c>
-      <c r="K44" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="L44" t="s">
         <v>60</v>
@@ -4057,7 +4062,7 @@
         <v>61</v>
       </c>
       <c r="P44" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Q44">
         <v>2</v>
@@ -4077,20 +4082,17 @@
       <c r="X44" t="s">
         <v>60</v>
       </c>
-      <c r="Y44" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z44" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA44" t="s">
-        <v>45</v>
+      <c r="AB44" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>204</v>
       </c>
       <c r="AD44" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AE44" s="3" t="s">
-        <v>60</v>
+        <v>205</v>
       </c>
     </row>
     <row r="45" spans="2:31" ht="45" x14ac:dyDescent="0.25">
@@ -4110,16 +4112,16 @@
         <v>35</v>
       </c>
       <c r="H45" t="s">
+        <v>164</v>
+      </c>
+      <c r="I45" t="s">
         <v>165</v>
       </c>
-      <c r="I45" t="s">
+      <c r="J45" t="s">
+        <v>57</v>
+      </c>
+      <c r="K45" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="J45" t="s">
-        <v>57</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="L45" t="s">
         <v>64</v>
@@ -4131,7 +4133,7 @@
         <v>65</v>
       </c>
       <c r="P45" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q45">
         <v>3</v>
@@ -4184,19 +4186,19 @@
         <v>35</v>
       </c>
       <c r="H46" t="s">
+        <v>164</v>
+      </c>
+      <c r="I46" t="s">
         <v>165</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
+        <v>57</v>
+      </c>
+      <c r="K46" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="J46" t="s">
-        <v>57</v>
-      </c>
-      <c r="K46" s="3" t="s">
+      <c r="L46" t="s">
         <v>167</v>
-      </c>
-      <c r="L46" t="s">
-        <v>168</v>
       </c>
       <c r="M46" t="s">
         <v>71</v>
@@ -4243,19 +4245,19 @@
         <v>35</v>
       </c>
       <c r="H47" t="s">
+        <v>164</v>
+      </c>
+      <c r="I47" t="s">
         <v>165</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
+        <v>57</v>
+      </c>
+      <c r="K47" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="J47" t="s">
-        <v>57</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="L47" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M47" t="s">
         <v>78</v>
@@ -4264,7 +4266,7 @@
         <v>79</v>
       </c>
       <c r="P47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q47">
         <v>5</v>
@@ -4294,16 +4296,16 @@
         <v>85</v>
       </c>
       <c r="AE47" s="3" t="s">
-        <v>86</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" t="s">
         <v>87</v>
       </c>
-      <c r="C48" t="s">
-        <v>88</v>
-      </c>
       <c r="D48" t="s">
         <v>33</v>
       </c>
@@ -4314,16 +4316,16 @@
         <v>35</v>
       </c>
       <c r="H48" t="s">
+        <v>170</v>
+      </c>
+      <c r="I48" t="s">
+        <v>165</v>
+      </c>
+      <c r="J48" t="s">
+        <v>57</v>
+      </c>
+      <c r="K48" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="I48" t="s">
-        <v>166</v>
-      </c>
-      <c r="J48" t="s">
-        <v>57</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="L48" t="s">
         <v>47</v>
@@ -4358,11 +4360,11 @@
     </row>
     <row r="49" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
+        <v>86</v>
+      </c>
+      <c r="C49" t="s">
         <v>87</v>
       </c>
-      <c r="C49" t="s">
-        <v>88</v>
-      </c>
       <c r="D49" t="s">
         <v>33</v>
       </c>
@@ -4373,16 +4375,16 @@
         <v>35</v>
       </c>
       <c r="H49" t="s">
+        <v>170</v>
+      </c>
+      <c r="I49" t="s">
+        <v>165</v>
+      </c>
+      <c r="J49" t="s">
+        <v>57</v>
+      </c>
+      <c r="K49" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="I49" t="s">
-        <v>166</v>
-      </c>
-      <c r="J49" t="s">
-        <v>57</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="L49" t="s">
         <v>60</v>
@@ -4394,7 +4396,7 @@
         <v>61</v>
       </c>
       <c r="P49" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Q49">
         <v>2</v>
@@ -4414,29 +4416,26 @@
       <c r="X49" t="s">
         <v>60</v>
       </c>
-      <c r="Y49" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z49" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA49" t="s">
-        <v>45</v>
+      <c r="AB49" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC49" t="s">
+        <v>204</v>
       </c>
       <c r="AD49" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AE49" s="3" t="s">
-        <v>60</v>
+        <v>206</v>
       </c>
     </row>
     <row r="50" spans="2:31" ht="45" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" t="s">
         <v>87</v>
       </c>
-      <c r="C50" t="s">
-        <v>88</v>
-      </c>
       <c r="D50" t="s">
         <v>33</v>
       </c>
@@ -4447,16 +4446,16 @@
         <v>35</v>
       </c>
       <c r="H50" t="s">
+        <v>170</v>
+      </c>
+      <c r="I50" t="s">
+        <v>165</v>
+      </c>
+      <c r="J50" t="s">
+        <v>57</v>
+      </c>
+      <c r="K50" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="I50" t="s">
-        <v>166</v>
-      </c>
-      <c r="J50" t="s">
-        <v>57</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="L50" t="s">
         <v>64</v>
@@ -4468,7 +4467,7 @@
         <v>65</v>
       </c>
       <c r="P50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q50">
         <v>3</v>
@@ -4506,11 +4505,11 @@
     </row>
     <row r="51" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" t="s">
         <v>87</v>
       </c>
-      <c r="C51" t="s">
-        <v>88</v>
-      </c>
       <c r="D51" t="s">
         <v>33</v>
       </c>
@@ -4521,28 +4520,28 @@
         <v>35</v>
       </c>
       <c r="H51" t="s">
+        <v>170</v>
+      </c>
+      <c r="I51" t="s">
+        <v>165</v>
+      </c>
+      <c r="J51" t="s">
+        <v>57</v>
+      </c>
+      <c r="K51" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="I51" t="s">
-        <v>166</v>
-      </c>
-      <c r="J51" t="s">
-        <v>57</v>
-      </c>
-      <c r="K51" s="3" t="s">
+      <c r="L51" t="s">
         <v>172</v>
-      </c>
-      <c r="L51" t="s">
-        <v>173</v>
       </c>
       <c r="M51" t="s">
         <v>71</v>
       </c>
       <c r="N51" t="s">
+        <v>90</v>
+      </c>
+      <c r="P51" t="s">
         <v>91</v>
-      </c>
-      <c r="P51" t="s">
-        <v>92</v>
       </c>
       <c r="Q51">
         <v>4</v>
@@ -4560,16 +4559,16 @@
         <v>75</v>
       </c>
       <c r="AE51" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" t="s">
         <v>87</v>
       </c>
-      <c r="C52" t="s">
-        <v>88</v>
-      </c>
       <c r="D52" t="s">
         <v>33</v>
       </c>
@@ -4580,28 +4579,28 @@
         <v>35</v>
       </c>
       <c r="H52" t="s">
+        <v>170</v>
+      </c>
+      <c r="I52" t="s">
+        <v>165</v>
+      </c>
+      <c r="J52" t="s">
+        <v>57</v>
+      </c>
+      <c r="K52" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="I52" t="s">
-        <v>166</v>
-      </c>
-      <c r="J52" t="s">
-        <v>57</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="L52" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M52" t="s">
         <v>78</v>
       </c>
       <c r="N52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P52" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q52">
         <v>5</v>
@@ -4622,10 +4621,10 @@
         <v>82</v>
       </c>
       <c r="Y52" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z52" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="Z52" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="AA52" t="s">
         <v>45</v>
@@ -4634,16 +4633,16 @@
         <v>85</v>
       </c>
       <c r="AE52" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" t="s">
         <v>100</v>
       </c>
-      <c r="C53" t="s">
-        <v>101</v>
-      </c>
       <c r="D53" t="s">
         <v>33</v>
       </c>
@@ -4654,16 +4653,16 @@
         <v>35</v>
       </c>
       <c r="H53" t="s">
+        <v>174</v>
+      </c>
+      <c r="I53" t="s">
+        <v>165</v>
+      </c>
+      <c r="J53" t="s">
+        <v>57</v>
+      </c>
+      <c r="K53" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="I53" t="s">
-        <v>166</v>
-      </c>
-      <c r="J53" t="s">
-        <v>57</v>
-      </c>
-      <c r="K53" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="L53" t="s">
         <v>47</v>
@@ -4698,11 +4697,11 @@
     </row>
     <row r="54" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" t="s">
         <v>100</v>
       </c>
-      <c r="C54" t="s">
-        <v>101</v>
-      </c>
       <c r="D54" t="s">
         <v>33</v>
       </c>
@@ -4713,16 +4712,16 @@
         <v>35</v>
       </c>
       <c r="H54" t="s">
+        <v>174</v>
+      </c>
+      <c r="I54" t="s">
+        <v>165</v>
+      </c>
+      <c r="J54" t="s">
+        <v>57</v>
+      </c>
+      <c r="K54" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="I54" t="s">
-        <v>166</v>
-      </c>
-      <c r="J54" t="s">
-        <v>57</v>
-      </c>
-      <c r="K54" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="L54" t="s">
         <v>60</v>
@@ -4734,7 +4733,7 @@
         <v>61</v>
       </c>
       <c r="P54" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Q54">
         <v>2</v>
@@ -4754,29 +4753,26 @@
       <c r="X54" t="s">
         <v>60</v>
       </c>
-      <c r="Y54" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z54" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA54" t="s">
-        <v>45</v>
+      <c r="AB54" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC54" t="s">
+        <v>204</v>
       </c>
       <c r="AD54" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AE54" s="3" t="s">
-        <v>60</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="2:31" ht="45" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" t="s">
         <v>100</v>
       </c>
-      <c r="C55" t="s">
-        <v>101</v>
-      </c>
       <c r="D55" t="s">
         <v>33</v>
       </c>
@@ -4787,16 +4783,16 @@
         <v>35</v>
       </c>
       <c r="H55" t="s">
+        <v>174</v>
+      </c>
+      <c r="I55" t="s">
+        <v>165</v>
+      </c>
+      <c r="J55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K55" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="I55" t="s">
-        <v>166</v>
-      </c>
-      <c r="J55" t="s">
-        <v>57</v>
-      </c>
-      <c r="K55" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="L55" t="s">
         <v>64</v>
@@ -4808,7 +4804,7 @@
         <v>65</v>
       </c>
       <c r="P55" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q55">
         <v>3</v>
@@ -4846,11 +4842,11 @@
     </row>
     <row r="56" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
+        <v>99</v>
+      </c>
+      <c r="C56" t="s">
         <v>100</v>
       </c>
-      <c r="C56" t="s">
-        <v>101</v>
-      </c>
       <c r="D56" t="s">
         <v>33</v>
       </c>
@@ -4861,28 +4857,28 @@
         <v>35</v>
       </c>
       <c r="H56" t="s">
+        <v>174</v>
+      </c>
+      <c r="I56" t="s">
+        <v>165</v>
+      </c>
+      <c r="J56" t="s">
+        <v>57</v>
+      </c>
+      <c r="K56" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="I56" t="s">
-        <v>166</v>
-      </c>
-      <c r="J56" t="s">
-        <v>57</v>
-      </c>
-      <c r="K56" s="3" t="s">
+      <c r="L56" t="s">
         <v>176</v>
-      </c>
-      <c r="L56" t="s">
-        <v>177</v>
       </c>
       <c r="M56" t="s">
         <v>71</v>
       </c>
       <c r="N56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q56">
         <v>4</v>
@@ -4900,16 +4896,16 @@
         <v>75</v>
       </c>
       <c r="AE56" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" t="s">
         <v>100</v>
       </c>
-      <c r="C57" t="s">
-        <v>101</v>
-      </c>
       <c r="D57" t="s">
         <v>33</v>
       </c>
@@ -4920,28 +4916,28 @@
         <v>35</v>
       </c>
       <c r="H57" t="s">
+        <v>174</v>
+      </c>
+      <c r="I57" t="s">
+        <v>165</v>
+      </c>
+      <c r="J57" t="s">
+        <v>57</v>
+      </c>
+      <c r="K57" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="I57" t="s">
-        <v>166</v>
-      </c>
-      <c r="J57" t="s">
-        <v>57</v>
-      </c>
-      <c r="K57" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="L57" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M57" t="s">
         <v>78</v>
       </c>
       <c r="N57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P57" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q57">
         <v>5</v>
@@ -4962,10 +4958,10 @@
         <v>82</v>
       </c>
       <c r="Y57" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z57" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="Z57" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="AA57" t="s">
         <v>45</v>
@@ -4974,16 +4970,16 @@
         <v>85</v>
       </c>
       <c r="AE57" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
+        <v>108</v>
+      </c>
+      <c r="C58" t="s">
         <v>109</v>
       </c>
-      <c r="C58" t="s">
-        <v>110</v>
-      </c>
       <c r="D58" t="s">
         <v>33</v>
       </c>
@@ -4994,16 +4990,16 @@
         <v>35</v>
       </c>
       <c r="H58" t="s">
+        <v>178</v>
+      </c>
+      <c r="I58" t="s">
+        <v>165</v>
+      </c>
+      <c r="J58" t="s">
+        <v>57</v>
+      </c>
+      <c r="K58" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="I58" t="s">
-        <v>166</v>
-      </c>
-      <c r="J58" t="s">
-        <v>57</v>
-      </c>
-      <c r="K58" s="3" t="s">
-        <v>180</v>
       </c>
       <c r="L58" t="s">
         <v>47</v>
@@ -5038,11 +5034,11 @@
     </row>
     <row r="59" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" t="s">
         <v>109</v>
       </c>
-      <c r="C59" t="s">
-        <v>110</v>
-      </c>
       <c r="D59" t="s">
         <v>33</v>
       </c>
@@ -5053,16 +5049,16 @@
         <v>35</v>
       </c>
       <c r="H59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I59" t="s">
+        <v>165</v>
+      </c>
+      <c r="J59" t="s">
+        <v>57</v>
+      </c>
+      <c r="K59" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="I59" t="s">
-        <v>166</v>
-      </c>
-      <c r="J59" t="s">
-        <v>57</v>
-      </c>
-      <c r="K59" s="3" t="s">
-        <v>180</v>
       </c>
       <c r="L59" t="s">
         <v>60</v>
@@ -5074,7 +5070,7 @@
         <v>61</v>
       </c>
       <c r="P59" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Q59">
         <v>2</v>
@@ -5094,29 +5090,26 @@
       <c r="X59" t="s">
         <v>60</v>
       </c>
-      <c r="Y59" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z59" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA59" t="s">
-        <v>45</v>
+      <c r="AB59" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC59" t="s">
+        <v>204</v>
       </c>
       <c r="AD59" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AE59" s="3" t="s">
-        <v>60</v>
+        <v>208</v>
       </c>
     </row>
     <row r="60" spans="2:31" ht="45" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
+        <v>108</v>
+      </c>
+      <c r="C60" t="s">
         <v>109</v>
       </c>
-      <c r="C60" t="s">
-        <v>110</v>
-      </c>
       <c r="D60" t="s">
         <v>33</v>
       </c>
@@ -5127,16 +5120,16 @@
         <v>35</v>
       </c>
       <c r="H60" t="s">
+        <v>178</v>
+      </c>
+      <c r="I60" t="s">
+        <v>165</v>
+      </c>
+      <c r="J60" t="s">
+        <v>57</v>
+      </c>
+      <c r="K60" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="I60" t="s">
-        <v>166</v>
-      </c>
-      <c r="J60" t="s">
-        <v>57</v>
-      </c>
-      <c r="K60" s="3" t="s">
-        <v>180</v>
       </c>
       <c r="L60" t="s">
         <v>64</v>
@@ -5148,7 +5141,7 @@
         <v>65</v>
       </c>
       <c r="P60" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q60">
         <v>3</v>
@@ -5186,11 +5179,11 @@
     </row>
     <row r="61" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
+        <v>108</v>
+      </c>
+      <c r="C61" t="s">
         <v>109</v>
       </c>
-      <c r="C61" t="s">
-        <v>110</v>
-      </c>
       <c r="D61" t="s">
         <v>33</v>
       </c>
@@ -5201,28 +5194,28 @@
         <v>35</v>
       </c>
       <c r="H61" t="s">
+        <v>178</v>
+      </c>
+      <c r="I61" t="s">
+        <v>165</v>
+      </c>
+      <c r="J61" t="s">
+        <v>57</v>
+      </c>
+      <c r="K61" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="I61" t="s">
-        <v>166</v>
-      </c>
-      <c r="J61" t="s">
-        <v>57</v>
-      </c>
-      <c r="K61" s="3" t="s">
+      <c r="L61" t="s">
         <v>180</v>
-      </c>
-      <c r="L61" t="s">
-        <v>181</v>
       </c>
       <c r="M61" t="s">
         <v>71</v>
       </c>
       <c r="N61" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P61" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q61">
         <v>4</v>
@@ -5240,16 +5233,16 @@
         <v>75</v>
       </c>
       <c r="AE61" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
+        <v>108</v>
+      </c>
+      <c r="C62" t="s">
         <v>109</v>
       </c>
-      <c r="C62" t="s">
-        <v>110</v>
-      </c>
       <c r="D62" t="s">
         <v>33</v>
       </c>
@@ -5260,28 +5253,28 @@
         <v>35</v>
       </c>
       <c r="H62" t="s">
+        <v>178</v>
+      </c>
+      <c r="I62" t="s">
+        <v>165</v>
+      </c>
+      <c r="J62" t="s">
+        <v>57</v>
+      </c>
+      <c r="K62" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="I62" t="s">
-        <v>166</v>
-      </c>
-      <c r="J62" t="s">
-        <v>57</v>
-      </c>
-      <c r="K62" s="3" t="s">
-        <v>180</v>
-      </c>
       <c r="L62" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M62" t="s">
         <v>78</v>
       </c>
       <c r="N62" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P62" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q62">
         <v>5</v>
@@ -5302,10 +5295,10 @@
         <v>82</v>
       </c>
       <c r="Y62" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z62" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="Z62" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="AA62" t="s">
         <v>45</v>
@@ -5314,16 +5307,16 @@
         <v>85</v>
       </c>
       <c r="AE62" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
+        <v>117</v>
+      </c>
+      <c r="C63" t="s">
         <v>118</v>
       </c>
-      <c r="C63" t="s">
-        <v>119</v>
-      </c>
       <c r="D63" t="s">
         <v>33</v>
       </c>
@@ -5334,16 +5327,16 @@
         <v>35</v>
       </c>
       <c r="H63" t="s">
+        <v>182</v>
+      </c>
+      <c r="I63" t="s">
+        <v>165</v>
+      </c>
+      <c r="J63" t="s">
+        <v>57</v>
+      </c>
+      <c r="K63" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="I63" t="s">
-        <v>166</v>
-      </c>
-      <c r="J63" t="s">
-        <v>57</v>
-      </c>
-      <c r="K63" s="3" t="s">
-        <v>184</v>
       </c>
       <c r="L63" t="s">
         <v>47</v>
@@ -5378,11 +5371,11 @@
     </row>
     <row r="64" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
+        <v>117</v>
+      </c>
+      <c r="C64" t="s">
         <v>118</v>
       </c>
-      <c r="C64" t="s">
-        <v>119</v>
-      </c>
       <c r="D64" t="s">
         <v>33</v>
       </c>
@@ -5393,16 +5386,16 @@
         <v>35</v>
       </c>
       <c r="H64" t="s">
+        <v>182</v>
+      </c>
+      <c r="I64" t="s">
+        <v>165</v>
+      </c>
+      <c r="J64" t="s">
+        <v>57</v>
+      </c>
+      <c r="K64" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="I64" t="s">
-        <v>166</v>
-      </c>
-      <c r="J64" t="s">
-        <v>57</v>
-      </c>
-      <c r="K64" s="3" t="s">
-        <v>184</v>
       </c>
       <c r="L64" t="s">
         <v>60</v>
@@ -5414,7 +5407,7 @@
         <v>61</v>
       </c>
       <c r="P64" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Q64">
         <v>2</v>
@@ -5434,29 +5427,26 @@
       <c r="X64" t="s">
         <v>60</v>
       </c>
-      <c r="Y64" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z64" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA64" t="s">
-        <v>45</v>
+      <c r="AB64" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC64" t="s">
+        <v>204</v>
       </c>
       <c r="AD64" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AE64" s="3" t="s">
-        <v>60</v>
+        <v>209</v>
       </c>
     </row>
     <row r="65" spans="2:31" ht="45" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
+        <v>117</v>
+      </c>
+      <c r="C65" t="s">
         <v>118</v>
       </c>
-      <c r="C65" t="s">
-        <v>119</v>
-      </c>
       <c r="D65" t="s">
         <v>33</v>
       </c>
@@ -5467,16 +5457,16 @@
         <v>35</v>
       </c>
       <c r="H65" t="s">
+        <v>182</v>
+      </c>
+      <c r="I65" t="s">
+        <v>165</v>
+      </c>
+      <c r="J65" t="s">
+        <v>57</v>
+      </c>
+      <c r="K65" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="I65" t="s">
-        <v>166</v>
-      </c>
-      <c r="J65" t="s">
-        <v>57</v>
-      </c>
-      <c r="K65" s="3" t="s">
-        <v>184</v>
       </c>
       <c r="L65" t="s">
         <v>64</v>
@@ -5488,7 +5478,7 @@
         <v>65</v>
       </c>
       <c r="P65" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q65">
         <v>3</v>
@@ -5526,11 +5516,11 @@
     </row>
     <row r="66" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
+        <v>117</v>
+      </c>
+      <c r="C66" t="s">
         <v>118</v>
       </c>
-      <c r="C66" t="s">
-        <v>119</v>
-      </c>
       <c r="D66" t="s">
         <v>33</v>
       </c>
@@ -5541,28 +5531,28 @@
         <v>35</v>
       </c>
       <c r="H66" t="s">
+        <v>182</v>
+      </c>
+      <c r="I66" t="s">
+        <v>165</v>
+      </c>
+      <c r="J66" t="s">
+        <v>57</v>
+      </c>
+      <c r="K66" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="I66" t="s">
-        <v>166</v>
-      </c>
-      <c r="J66" t="s">
-        <v>57</v>
-      </c>
-      <c r="K66" s="3" t="s">
+      <c r="L66" t="s">
         <v>184</v>
-      </c>
-      <c r="L66" t="s">
-        <v>185</v>
       </c>
       <c r="M66" t="s">
         <v>71</v>
       </c>
       <c r="N66" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P66" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q66">
         <v>4</v>
@@ -5580,16 +5570,16 @@
         <v>75</v>
       </c>
       <c r="AE66" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="67" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
+        <v>117</v>
+      </c>
+      <c r="C67" t="s">
         <v>118</v>
       </c>
-      <c r="C67" t="s">
-        <v>119</v>
-      </c>
       <c r="D67" t="s">
         <v>33</v>
       </c>
@@ -5600,28 +5590,28 @@
         <v>35</v>
       </c>
       <c r="H67" t="s">
+        <v>182</v>
+      </c>
+      <c r="I67" t="s">
+        <v>165</v>
+      </c>
+      <c r="J67" t="s">
+        <v>57</v>
+      </c>
+      <c r="K67" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="I67" t="s">
-        <v>166</v>
-      </c>
-      <c r="J67" t="s">
-        <v>57</v>
-      </c>
-      <c r="K67" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="L67" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M67" t="s">
         <v>78</v>
       </c>
       <c r="N67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P67" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q67">
         <v>5</v>
@@ -5642,10 +5632,10 @@
         <v>82</v>
       </c>
       <c r="Y67" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z67" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="Z67" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="AA67" t="s">
         <v>45</v>
@@ -5654,16 +5644,16 @@
         <v>85</v>
       </c>
       <c r="AE67" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
+        <v>126</v>
+      </c>
+      <c r="C68" t="s">
         <v>127</v>
       </c>
-      <c r="C68" t="s">
-        <v>128</v>
-      </c>
       <c r="D68" t="s">
         <v>33</v>
       </c>
@@ -5674,16 +5664,16 @@
         <v>35</v>
       </c>
       <c r="H68" t="s">
+        <v>186</v>
+      </c>
+      <c r="I68" t="s">
+        <v>165</v>
+      </c>
+      <c r="J68" t="s">
+        <v>57</v>
+      </c>
+      <c r="K68" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="I68" t="s">
-        <v>166</v>
-      </c>
-      <c r="J68" t="s">
-        <v>57</v>
-      </c>
-      <c r="K68" s="3" t="s">
-        <v>188</v>
       </c>
       <c r="L68" t="s">
         <v>47</v>
@@ -5718,11 +5708,11 @@
     </row>
     <row r="69" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
+        <v>126</v>
+      </c>
+      <c r="C69" t="s">
         <v>127</v>
       </c>
-      <c r="C69" t="s">
-        <v>128</v>
-      </c>
       <c r="D69" t="s">
         <v>33</v>
       </c>
@@ -5733,16 +5723,16 @@
         <v>35</v>
       </c>
       <c r="H69" t="s">
+        <v>186</v>
+      </c>
+      <c r="I69" t="s">
+        <v>165</v>
+      </c>
+      <c r="J69" t="s">
+        <v>57</v>
+      </c>
+      <c r="K69" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="I69" t="s">
-        <v>166</v>
-      </c>
-      <c r="J69" t="s">
-        <v>57</v>
-      </c>
-      <c r="K69" s="3" t="s">
-        <v>188</v>
       </c>
       <c r="L69" t="s">
         <v>60</v>
@@ -5754,7 +5744,7 @@
         <v>61</v>
       </c>
       <c r="P69" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Q69">
         <v>2</v>
@@ -5774,29 +5764,26 @@
       <c r="X69" t="s">
         <v>60</v>
       </c>
-      <c r="Y69" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z69" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA69" t="s">
-        <v>45</v>
+      <c r="AB69" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC69" t="s">
+        <v>204</v>
       </c>
       <c r="AD69" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AE69" s="3" t="s">
-        <v>60</v>
+        <v>210</v>
       </c>
     </row>
     <row r="70" spans="2:31" ht="45" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
+        <v>126</v>
+      </c>
+      <c r="C70" t="s">
         <v>127</v>
       </c>
-      <c r="C70" t="s">
-        <v>128</v>
-      </c>
       <c r="D70" t="s">
         <v>33</v>
       </c>
@@ -5807,16 +5794,16 @@
         <v>35</v>
       </c>
       <c r="H70" t="s">
+        <v>186</v>
+      </c>
+      <c r="I70" t="s">
+        <v>165</v>
+      </c>
+      <c r="J70" t="s">
+        <v>57</v>
+      </c>
+      <c r="K70" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="I70" t="s">
-        <v>166</v>
-      </c>
-      <c r="J70" t="s">
-        <v>57</v>
-      </c>
-      <c r="K70" s="3" t="s">
-        <v>188</v>
       </c>
       <c r="L70" t="s">
         <v>64</v>
@@ -5828,7 +5815,7 @@
         <v>65</v>
       </c>
       <c r="P70" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q70">
         <v>3</v>
@@ -5866,11 +5853,11 @@
     </row>
     <row r="71" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
+        <v>126</v>
+      </c>
+      <c r="C71" t="s">
         <v>127</v>
       </c>
-      <c r="C71" t="s">
-        <v>128</v>
-      </c>
       <c r="D71" t="s">
         <v>33</v>
       </c>
@@ -5881,28 +5868,28 @@
         <v>35</v>
       </c>
       <c r="H71" t="s">
+        <v>186</v>
+      </c>
+      <c r="I71" t="s">
+        <v>165</v>
+      </c>
+      <c r="J71" t="s">
+        <v>57</v>
+      </c>
+      <c r="K71" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="I71" t="s">
-        <v>166</v>
-      </c>
-      <c r="J71" t="s">
-        <v>57</v>
-      </c>
-      <c r="K71" s="3" t="s">
+      <c r="L71" t="s">
         <v>188</v>
-      </c>
-      <c r="L71" t="s">
-        <v>189</v>
       </c>
       <c r="M71" t="s">
         <v>71</v>
       </c>
       <c r="N71" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P71" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q71">
         <v>4</v>
@@ -5920,16 +5907,16 @@
         <v>75</v>
       </c>
       <c r="AE71" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="72" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
+        <v>126</v>
+      </c>
+      <c r="C72" t="s">
         <v>127</v>
       </c>
-      <c r="C72" t="s">
-        <v>128</v>
-      </c>
       <c r="D72" t="s">
         <v>33</v>
       </c>
@@ -5940,28 +5927,28 @@
         <v>35</v>
       </c>
       <c r="H72" t="s">
+        <v>186</v>
+      </c>
+      <c r="I72" t="s">
+        <v>165</v>
+      </c>
+      <c r="J72" t="s">
+        <v>57</v>
+      </c>
+      <c r="K72" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="I72" t="s">
-        <v>166</v>
-      </c>
-      <c r="J72" t="s">
-        <v>57</v>
-      </c>
-      <c r="K72" s="3" t="s">
-        <v>188</v>
-      </c>
       <c r="L72" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M72" t="s">
         <v>78</v>
       </c>
       <c r="N72" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P72" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q72">
         <v>5</v>
@@ -5982,10 +5969,10 @@
         <v>82</v>
       </c>
       <c r="Y72" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z72" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="Z72" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="AA72" t="s">
         <v>45</v>
@@ -5994,16 +5981,16 @@
         <v>85</v>
       </c>
       <c r="AE72" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="73" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
+        <v>135</v>
+      </c>
+      <c r="C73" t="s">
         <v>136</v>
       </c>
-      <c r="C73" t="s">
-        <v>137</v>
-      </c>
       <c r="D73" t="s">
         <v>33</v>
       </c>
@@ -6014,16 +6001,16 @@
         <v>35</v>
       </c>
       <c r="H73" t="s">
+        <v>190</v>
+      </c>
+      <c r="I73" t="s">
+        <v>165</v>
+      </c>
+      <c r="J73" t="s">
+        <v>57</v>
+      </c>
+      <c r="K73" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="I73" t="s">
-        <v>166</v>
-      </c>
-      <c r="J73" t="s">
-        <v>57</v>
-      </c>
-      <c r="K73" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="L73" t="s">
         <v>47</v>
@@ -6058,11 +6045,11 @@
     </row>
     <row r="74" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
+        <v>135</v>
+      </c>
+      <c r="C74" t="s">
         <v>136</v>
       </c>
-      <c r="C74" t="s">
-        <v>137</v>
-      </c>
       <c r="D74" t="s">
         <v>33</v>
       </c>
@@ -6073,16 +6060,16 @@
         <v>35</v>
       </c>
       <c r="H74" t="s">
+        <v>190</v>
+      </c>
+      <c r="I74" t="s">
+        <v>165</v>
+      </c>
+      <c r="J74" t="s">
+        <v>57</v>
+      </c>
+      <c r="K74" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="I74" t="s">
-        <v>166</v>
-      </c>
-      <c r="J74" t="s">
-        <v>57</v>
-      </c>
-      <c r="K74" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="L74" t="s">
         <v>60</v>
@@ -6094,7 +6081,7 @@
         <v>61</v>
       </c>
       <c r="P74" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="Q74">
         <v>2</v>
@@ -6114,29 +6101,26 @@
       <c r="X74" t="s">
         <v>60</v>
       </c>
-      <c r="Y74" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z74" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA74" t="s">
-        <v>45</v>
+      <c r="AB74" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AC74" t="s">
+        <v>204</v>
       </c>
       <c r="AD74" s="3" t="s">
         <v>60</v>
       </c>
       <c r="AE74" s="3" t="s">
-        <v>60</v>
+        <v>211</v>
       </c>
     </row>
     <row r="75" spans="2:31" ht="45" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
+        <v>135</v>
+      </c>
+      <c r="C75" t="s">
         <v>136</v>
       </c>
-      <c r="C75" t="s">
-        <v>137</v>
-      </c>
       <c r="D75" t="s">
         <v>33</v>
       </c>
@@ -6147,16 +6131,16 @@
         <v>35</v>
       </c>
       <c r="H75" t="s">
+        <v>190</v>
+      </c>
+      <c r="I75" t="s">
+        <v>165</v>
+      </c>
+      <c r="J75" t="s">
+        <v>57</v>
+      </c>
+      <c r="K75" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="I75" t="s">
-        <v>166</v>
-      </c>
-      <c r="J75" t="s">
-        <v>57</v>
-      </c>
-      <c r="K75" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="L75" t="s">
         <v>64</v>
@@ -6168,7 +6152,7 @@
         <v>65</v>
       </c>
       <c r="P75" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q75">
         <v>3</v>
@@ -6206,11 +6190,11 @@
     </row>
     <row r="76" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
+        <v>135</v>
+      </c>
+      <c r="C76" t="s">
         <v>136</v>
       </c>
-      <c r="C76" t="s">
-        <v>137</v>
-      </c>
       <c r="D76" t="s">
         <v>33</v>
       </c>
@@ -6221,28 +6205,28 @@
         <v>35</v>
       </c>
       <c r="H76" t="s">
+        <v>190</v>
+      </c>
+      <c r="I76" t="s">
+        <v>165</v>
+      </c>
+      <c r="J76" t="s">
+        <v>57</v>
+      </c>
+      <c r="K76" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="I76" t="s">
-        <v>166</v>
-      </c>
-      <c r="J76" t="s">
-        <v>57</v>
-      </c>
-      <c r="K76" s="3" t="s">
+      <c r="L76" t="s">
         <v>192</v>
-      </c>
-      <c r="L76" t="s">
-        <v>193</v>
       </c>
       <c r="M76" t="s">
         <v>71</v>
       </c>
       <c r="N76" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P76" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q76">
         <v>4</v>
@@ -6260,16 +6244,16 @@
         <v>75</v>
       </c>
       <c r="AE76" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
+        <v>135</v>
+      </c>
+      <c r="C77" t="s">
         <v>136</v>
       </c>
-      <c r="C77" t="s">
-        <v>137</v>
-      </c>
       <c r="D77" t="s">
         <v>33</v>
       </c>
@@ -6280,28 +6264,28 @@
         <v>35</v>
       </c>
       <c r="H77" t="s">
+        <v>190</v>
+      </c>
+      <c r="I77" t="s">
+        <v>165</v>
+      </c>
+      <c r="J77" t="s">
+        <v>57</v>
+      </c>
+      <c r="K77" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="I77" t="s">
-        <v>166</v>
-      </c>
-      <c r="J77" t="s">
-        <v>57</v>
-      </c>
-      <c r="K77" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="L77" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M77" t="s">
         <v>78</v>
       </c>
       <c r="N77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P77" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q77">
         <v>5</v>
@@ -6322,10 +6306,10 @@
         <v>82</v>
       </c>
       <c r="Y77" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z77" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="Z77" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="AA77" t="s">
         <v>45</v>
@@ -6334,16 +6318,16 @@
         <v>85</v>
       </c>
       <c r="AE77" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="78" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
+        <v>144</v>
+      </c>
+      <c r="C78" t="s">
         <v>145</v>
       </c>
-      <c r="C78" t="s">
-        <v>146</v>
-      </c>
       <c r="D78" t="s">
         <v>33</v>
       </c>
@@ -6354,16 +6338,16 @@
         <v>35</v>
       </c>
       <c r="H78" t="s">
+        <v>194</v>
+      </c>
+      <c r="I78" t="s">
+        <v>165</v>
+      </c>
+      <c r="J78" t="s">
+        <v>57</v>
+      </c>
+      <c r="K78" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="I78" t="s">
-        <v>166</v>
-      </c>
-      <c r="J78" t="s">
-        <v>57</v>
-      </c>
-      <c r="K78" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="L78" t="s">
         <v>47</v>
@@ -6398,11 +6382,11 @@
     </row>
     <row r="79" spans="2:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
+        <v>144</v>
+      </c>
+      <c r="C79" t="s">
         <v>145</v>
       </c>
-      <c r="C79" t="s">
-        <v>146</v>
-      </c>
       <c r="D79" t="s">
         <v>33</v>
       </c>
@@ -6413,28 +6397,28 @@
         <v>35</v>
       </c>
       <c r="H79" t="s">
+        <v>194</v>
+      </c>
+      <c r="I79" t="s">
+        <v>165</v>
+      </c>
+      <c r="J79" t="s">
+        <v>57</v>
+      </c>
+      <c r="K79" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="I79" t="s">
-        <v>166</v>
-      </c>
-      <c r="J79" t="s">
-        <v>57</v>
-      </c>
-      <c r="K79" s="3" t="s">
+      <c r="L79" t="s">
         <v>196</v>
-      </c>
-      <c r="L79" t="s">
-        <v>197</v>
       </c>
       <c r="M79" t="s">
         <v>71</v>
       </c>
       <c r="N79" t="s">
+        <v>149</v>
+      </c>
+      <c r="P79" t="s">
         <v>150</v>
-      </c>
-      <c r="P79" t="s">
-        <v>151</v>
       </c>
       <c r="Q79">
         <v>2</v>
@@ -6449,16 +6433,16 @@
         <v>50</v>
       </c>
       <c r="W79" t="s">
+        <v>151</v>
+      </c>
+      <c r="X79" t="s">
         <v>152</v>
       </c>
-      <c r="X79" t="s">
+      <c r="Y79" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="Y79" s="3" t="s">
+      <c r="Z79" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="Z79" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="AA79" t="s">
         <v>45</v>
@@ -6467,16 +6451,16 @@
         <v>75</v>
       </c>
       <c r="AE79" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="80" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
+        <v>144</v>
+      </c>
+      <c r="C80" t="s">
         <v>145</v>
       </c>
-      <c r="C80" t="s">
-        <v>146</v>
-      </c>
       <c r="D80" t="s">
         <v>33</v>
       </c>
@@ -6487,28 +6471,28 @@
         <v>35</v>
       </c>
       <c r="H80" t="s">
+        <v>194</v>
+      </c>
+      <c r="I80" t="s">
+        <v>165</v>
+      </c>
+      <c r="J80" t="s">
+        <v>57</v>
+      </c>
+      <c r="K80" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="I80" t="s">
-        <v>166</v>
-      </c>
-      <c r="J80" t="s">
-        <v>57</v>
-      </c>
-      <c r="K80" s="3" t="s">
-        <v>196</v>
-      </c>
       <c r="L80" t="s">
+        <v>156</v>
+      </c>
+      <c r="M80" t="s">
+        <v>156</v>
+      </c>
+      <c r="N80" t="s">
         <v>157</v>
       </c>
-      <c r="M80" t="s">
-        <v>157</v>
-      </c>
-      <c r="N80" t="s">
+      <c r="P80" t="s">
         <v>158</v>
-      </c>
-      <c r="P80" t="s">
-        <v>159</v>
       </c>
       <c r="Q80">
         <v>3</v>
@@ -6538,19 +6522,19 @@
         <v>45</v>
       </c>
       <c r="AD80" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AE80" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="81" spans="2:31" ht="75" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
+        <v>144</v>
+      </c>
+      <c r="C81" t="s">
         <v>145</v>
       </c>
-      <c r="C81" t="s">
-        <v>146</v>
-      </c>
       <c r="D81" t="s">
         <v>33</v>
       </c>
@@ -6561,28 +6545,28 @@
         <v>35</v>
       </c>
       <c r="H81" t="s">
+        <v>194</v>
+      </c>
+      <c r="I81" t="s">
+        <v>165</v>
+      </c>
+      <c r="J81" t="s">
+        <v>57</v>
+      </c>
+      <c r="K81" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="I81" t="s">
-        <v>166</v>
-      </c>
-      <c r="J81" t="s">
-        <v>57</v>
-      </c>
-      <c r="K81" s="3" t="s">
-        <v>196</v>
-      </c>
       <c r="L81" t="s">
+        <v>159</v>
+      </c>
+      <c r="M81" t="s">
+        <v>159</v>
+      </c>
+      <c r="N81" t="s">
         <v>160</v>
       </c>
-      <c r="M81" t="s">
-        <v>160</v>
-      </c>
-      <c r="N81" t="s">
-        <v>161</v>
-      </c>
       <c r="P81" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q81">
         <v>4</v>
@@ -6597,25 +6581,25 @@
         <v>50</v>
       </c>
       <c r="W81" t="s">
+        <v>162</v>
+      </c>
+      <c r="X81" t="s">
         <v>163</v>
       </c>
-      <c r="X81" t="s">
-        <v>164</v>
-      </c>
       <c r="Y81" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="Z81" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AA81" t="s">
         <v>45</v>
       </c>
       <c r="AD81" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AE81" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated EG to remove dec_id for --TEST, updated RRAG dec_id
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_EG_Local.xlsx
+++ b/curation/draft/collection/collection_specialization_EG_Local.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C643F4BB-C504-B64D-9181-6227A3310672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842463DE-8AE3-934F-9A76-8750F678E0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2800" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3760" yWindow="4500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_EG" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4687" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4667" uniqueCount="376">
   <si>
     <t>package_date</t>
   </si>
@@ -1164,6 +1164,9 @@
   </si>
   <si>
     <t>derivation_description</t>
+  </si>
+  <si>
+    <t>RRAG_EGORRES</t>
   </si>
 </sst>
 </file>
@@ -1608,9 +1611,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O102" sqref="O102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3067,9 +3070,6 @@
       <c r="N22" t="s">
         <v>186</v>
       </c>
-      <c r="O22" t="s">
-        <v>191</v>
-      </c>
       <c r="Q22" t="s">
         <v>187</v>
       </c>
@@ -3525,9 +3525,6 @@
       <c r="N29" t="s">
         <v>186</v>
       </c>
-      <c r="O29" t="s">
-        <v>191</v>
-      </c>
       <c r="Q29" t="s">
         <v>187</v>
       </c>
@@ -3983,9 +3980,6 @@
       <c r="N36" t="s">
         <v>186</v>
       </c>
-      <c r="O36" t="s">
-        <v>191</v>
-      </c>
       <c r="Q36" t="s">
         <v>187</v>
       </c>
@@ -4441,9 +4435,6 @@
       <c r="N43" t="s">
         <v>186</v>
       </c>
-      <c r="O43" t="s">
-        <v>191</v>
-      </c>
       <c r="Q43" t="s">
         <v>187</v>
       </c>
@@ -4899,9 +4890,6 @@
       <c r="N50" t="s">
         <v>186</v>
       </c>
-      <c r="O50" t="s">
-        <v>191</v>
-      </c>
       <c r="Q50" t="s">
         <v>187</v>
       </c>
@@ -5162,11 +5150,8 @@
       <c r="N54" t="s">
         <v>186</v>
       </c>
-      <c r="O54" t="s">
-        <v>191</v>
-      </c>
       <c r="Q54" t="s">
-        <v>148</v>
+        <v>187</v>
       </c>
       <c r="R54">
         <v>2</v>
@@ -8346,9 +8331,6 @@
       <c r="N101" t="s">
         <v>186</v>
       </c>
-      <c r="O101" t="s">
-        <v>191</v>
-      </c>
       <c r="Q101" t="s">
         <v>187</v>
       </c>
@@ -8418,7 +8400,7 @@
         <v>65</v>
       </c>
       <c r="O102" t="s">
-        <v>370</v>
+        <v>82</v>
       </c>
       <c r="Q102" t="s">
         <v>188</v>
@@ -8747,10 +8729,10 @@
         <v>222</v>
       </c>
       <c r="M107" t="s">
-        <v>223</v>
+        <v>375</v>
       </c>
       <c r="N107" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="O107" t="s">
         <v>82</v>
@@ -9136,9 +9118,6 @@
       </c>
       <c r="N113" t="s">
         <v>186</v>
-      </c>
-      <c r="O113" t="s">
-        <v>191</v>
       </c>
       <c r="Q113" t="s">
         <v>187</v>
@@ -10182,9 +10161,6 @@
       <c r="N129" t="s">
         <v>186</v>
       </c>
-      <c r="O129" t="s">
-        <v>191</v>
-      </c>
       <c r="Q129" t="s">
         <v>187</v>
       </c>
@@ -10829,9 +10805,6 @@
       <c r="N139" t="s">
         <v>186</v>
       </c>
-      <c r="O139" t="s">
-        <v>191</v>
-      </c>
       <c r="Q139" t="s">
         <v>187</v>
       </c>
@@ -11476,9 +11449,6 @@
       <c r="N149" t="s">
         <v>186</v>
       </c>
-      <c r="O149" t="s">
-        <v>191</v>
-      </c>
       <c r="Q149" t="s">
         <v>187</v>
       </c>
@@ -12123,9 +12093,6 @@
       <c r="N159" t="s">
         <v>186</v>
       </c>
-      <c r="O159" t="s">
-        <v>191</v>
-      </c>
       <c r="Q159" t="s">
         <v>187</v>
       </c>
@@ -12770,9 +12737,6 @@
       <c r="N169" t="s">
         <v>186</v>
       </c>
-      <c r="O169" t="s">
-        <v>191</v>
-      </c>
       <c r="Q169" t="s">
         <v>187</v>
       </c>
@@ -13417,9 +13381,6 @@
       <c r="N179" t="s">
         <v>186</v>
       </c>
-      <c r="O179" t="s">
-        <v>191</v>
-      </c>
       <c r="Q179" t="s">
         <v>187</v>
       </c>
@@ -14064,9 +14025,6 @@
       <c r="N189" t="s">
         <v>186</v>
       </c>
-      <c r="O189" t="s">
-        <v>191</v>
-      </c>
       <c r="Q189" t="s">
         <v>187</v>
       </c>
@@ -14711,9 +14669,6 @@
       <c r="N199" t="s">
         <v>186</v>
       </c>
-      <c r="O199" t="s">
-        <v>191</v>
-      </c>
       <c r="Q199" t="s">
         <v>187</v>
       </c>
@@ -15358,9 +15313,6 @@
       <c r="N209" t="s">
         <v>186</v>
       </c>
-      <c r="O209" t="s">
-        <v>191</v>
-      </c>
       <c r="Q209" t="s">
         <v>187</v>
       </c>
@@ -16005,9 +15957,6 @@
       <c r="N219" t="s">
         <v>186</v>
       </c>
-      <c r="O219" t="s">
-        <v>191</v>
-      </c>
       <c r="Q219" t="s">
         <v>187</v>
       </c>
@@ -16652,9 +16601,6 @@
       <c r="N229" t="s">
         <v>186</v>
       </c>
-      <c r="O229" t="s">
-        <v>191</v>
-      </c>
       <c r="Q229" t="s">
         <v>187</v>
       </c>
@@ -17298,9 +17244,6 @@
       </c>
       <c r="N239" t="s">
         <v>186</v>
-      </c>
-      <c r="O239" t="s">
-        <v>191</v>
       </c>
       <c r="Q239" t="s">
         <v>187</v>

</xml_diff>